<commit_message>
Schaltung un d Board verandert
</commit_message>
<xml_diff>
--- a/Informationen/Fahradcomputer_mk2_Materialliste.xlsx
+++ b/Informationen/Fahradcomputer_mk2_Materialliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Bateilname:</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>120pF</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -454,7 +457,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -508,6 +511,9 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -610,16 +616,22 @@
       <c r="B16">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>22</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -627,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -635,7 +647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -643,15 +655,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="E21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -659,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -667,20 +682,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
         <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>